<commit_message>
Uploaded current version of clean data (filled na values)
</commit_message>
<xml_diff>
--- a/clean_data.xlsx
+++ b/clean_data.xlsx
@@ -1729,6 +1729,12 @@
       <c r="K4">
         <v>9</v>
       </c>
+      <c r="L4">
+        <v>3.638888888888889</v>
+      </c>
+      <c r="M4">
+        <v>0.5888888888888889</v>
+      </c>
       <c r="N4" t="s">
         <v>286</v>
       </c>
@@ -1867,6 +1873,9 @@
       <c r="K7">
         <v>8</v>
       </c>
+      <c r="L7">
+        <v>3.638888888888889</v>
+      </c>
       <c r="M7">
         <v>0</v>
       </c>
@@ -1917,6 +1926,9 @@
       <c r="L8">
         <v>2</v>
       </c>
+      <c r="M8">
+        <v>0.5888888888888889</v>
+      </c>
       <c r="N8" t="s">
         <v>286</v>
       </c>
@@ -2308,6 +2320,9 @@
       <c r="K16">
         <v>138</v>
       </c>
+      <c r="L16">
+        <v>3.638888888888889</v>
+      </c>
       <c r="M16">
         <v>0</v>
       </c>
@@ -2402,6 +2417,9 @@
       <c r="K18">
         <v>111</v>
       </c>
+      <c r="L18">
+        <v>3.638888888888889</v>
+      </c>
       <c r="M18">
         <v>3</v>
       </c>
@@ -2496,6 +2514,9 @@
       <c r="K20">
         <v>57</v>
       </c>
+      <c r="L20">
+        <v>3.638888888888889</v>
+      </c>
       <c r="M20">
         <v>1</v>
       </c>
@@ -2543,6 +2564,9 @@
       <c r="K21">
         <v>17</v>
       </c>
+      <c r="L21">
+        <v>3.638888888888889</v>
+      </c>
       <c r="M21">
         <v>0</v>
       </c>
@@ -2587,6 +2611,9 @@
       <c r="K22">
         <v>7</v>
       </c>
+      <c r="L22">
+        <v>3.638888888888889</v>
+      </c>
       <c r="M22">
         <v>0</v>
       </c>
@@ -2631,6 +2658,9 @@
       <c r="K23">
         <v>25</v>
       </c>
+      <c r="L23">
+        <v>3.638888888888889</v>
+      </c>
       <c r="M23">
         <v>0</v>
       </c>
@@ -2672,6 +2702,9 @@
       <c r="K24">
         <v>25</v>
       </c>
+      <c r="L24">
+        <v>3.638888888888889</v>
+      </c>
       <c r="M24">
         <v>0</v>
       </c>
@@ -2716,6 +2749,9 @@
       <c r="K25">
         <v>10</v>
       </c>
+      <c r="L25">
+        <v>3.638888888888889</v>
+      </c>
       <c r="M25">
         <v>1</v>
       </c>
@@ -2763,6 +2799,9 @@
       <c r="K26">
         <v>28</v>
       </c>
+      <c r="L26">
+        <v>3.638888888888889</v>
+      </c>
       <c r="M26">
         <v>3</v>
       </c>
@@ -2810,6 +2849,9 @@
       <c r="K27">
         <v>24</v>
       </c>
+      <c r="L27">
+        <v>3.638888888888889</v>
+      </c>
       <c r="M27">
         <v>0</v>
       </c>
@@ -2857,6 +2899,9 @@
       <c r="K28">
         <v>8</v>
       </c>
+      <c r="L28">
+        <v>3.638888888888889</v>
+      </c>
       <c r="M28">
         <v>0</v>
       </c>
@@ -2901,6 +2946,9 @@
       <c r="K29">
         <v>4</v>
       </c>
+      <c r="L29">
+        <v>3.638888888888889</v>
+      </c>
       <c r="M29">
         <v>0</v>
       </c>
@@ -2948,6 +2996,9 @@
       <c r="K30">
         <v>4</v>
       </c>
+      <c r="L30">
+        <v>3.638888888888889</v>
+      </c>
       <c r="M30">
         <v>0</v>
       </c>
@@ -2995,6 +3046,9 @@
       <c r="K31">
         <v>22</v>
       </c>
+      <c r="L31">
+        <v>3.638888888888889</v>
+      </c>
       <c r="M31">
         <v>0</v>
       </c>
@@ -3042,6 +3096,9 @@
       <c r="K32">
         <v>17</v>
       </c>
+      <c r="L32">
+        <v>3.638888888888889</v>
+      </c>
       <c r="M32">
         <v>0</v>
       </c>
@@ -3089,6 +3146,9 @@
       <c r="K33">
         <v>17</v>
       </c>
+      <c r="L33">
+        <v>3.638888888888889</v>
+      </c>
       <c r="M33">
         <v>0</v>
       </c>
@@ -3136,6 +3196,9 @@
       <c r="K34">
         <v>111</v>
       </c>
+      <c r="L34">
+        <v>3.638888888888889</v>
+      </c>
       <c r="M34">
         <v>3</v>
       </c>
@@ -3180,6 +3243,9 @@
       <c r="K35">
         <v>3</v>
       </c>
+      <c r="L35">
+        <v>3.638888888888889</v>
+      </c>
       <c r="M35">
         <v>0</v>
       </c>
@@ -3227,6 +3293,9 @@
       <c r="K36">
         <v>2</v>
       </c>
+      <c r="L36">
+        <v>3.638888888888889</v>
+      </c>
       <c r="M36">
         <v>2</v>
       </c>
@@ -3274,6 +3343,9 @@
       <c r="K37">
         <v>2</v>
       </c>
+      <c r="L37">
+        <v>3.638888888888889</v>
+      </c>
       <c r="M37">
         <v>2</v>
       </c>
@@ -3321,6 +3393,12 @@
       <c r="K38">
         <v>21</v>
       </c>
+      <c r="L38">
+        <v>3.638888888888889</v>
+      </c>
+      <c r="M38">
+        <v>0.5888888888888889</v>
+      </c>
       <c r="N38" t="s">
         <v>296</v>
       </c>
@@ -3362,6 +3440,9 @@
       <c r="K39">
         <v>11</v>
       </c>
+      <c r="L39">
+        <v>3.638888888888889</v>
+      </c>
       <c r="M39">
         <v>2</v>
       </c>
@@ -3406,6 +3487,9 @@
       <c r="K40">
         <v>9</v>
       </c>
+      <c r="L40">
+        <v>3.638888888888889</v>
+      </c>
       <c r="M40">
         <v>2</v>
       </c>
@@ -3453,6 +3537,9 @@
       <c r="K41">
         <v>69</v>
       </c>
+      <c r="L41">
+        <v>3.638888888888889</v>
+      </c>
       <c r="M41">
         <v>0</v>
       </c>
@@ -3647,6 +3734,9 @@
       <c r="K45">
         <v>72</v>
       </c>
+      <c r="L45">
+        <v>3.638888888888889</v>
+      </c>
       <c r="M45">
         <v>2</v>
       </c>
@@ -3744,6 +3834,12 @@
       <c r="K47">
         <v>21</v>
       </c>
+      <c r="L47">
+        <v>3.638888888888889</v>
+      </c>
+      <c r="M47">
+        <v>0.5888888888888889</v>
+      </c>
       <c r="N47" t="s">
         <v>297</v>
       </c>
@@ -4032,6 +4128,12 @@
       <c r="K53">
         <v>13</v>
       </c>
+      <c r="L53">
+        <v>3.638888888888889</v>
+      </c>
+      <c r="M53">
+        <v>0.5888888888888889</v>
+      </c>
       <c r="N53" t="s">
         <v>286</v>
       </c>
@@ -4126,6 +4228,9 @@
       <c r="K55">
         <v>3</v>
       </c>
+      <c r="L55">
+        <v>3.638888888888889</v>
+      </c>
       <c r="M55">
         <v>0</v>
       </c>
@@ -4223,6 +4328,9 @@
       <c r="K57">
         <v>2</v>
       </c>
+      <c r="L57">
+        <v>3.638888888888889</v>
+      </c>
       <c r="M57">
         <v>0</v>
       </c>
@@ -4270,6 +4378,9 @@
       <c r="K58">
         <v>8</v>
       </c>
+      <c r="L58">
+        <v>3.638888888888889</v>
+      </c>
       <c r="M58">
         <v>0</v>
       </c>
@@ -4317,6 +4428,9 @@
       <c r="K59">
         <v>8</v>
       </c>
+      <c r="L59">
+        <v>3.638888888888889</v>
+      </c>
       <c r="M59">
         <v>0</v>
       </c>
@@ -4361,6 +4475,12 @@
       <c r="K60">
         <v>7</v>
       </c>
+      <c r="L60">
+        <v>3.638888888888889</v>
+      </c>
+      <c r="M60">
+        <v>0.5888888888888889</v>
+      </c>
       <c r="N60" t="s">
         <v>286</v>
       </c>
@@ -4402,6 +4522,9 @@
       <c r="K61">
         <v>3</v>
       </c>
+      <c r="L61">
+        <v>3.638888888888889</v>
+      </c>
       <c r="M61">
         <v>0</v>
       </c>
@@ -4449,6 +4572,9 @@
       <c r="K62">
         <v>7</v>
       </c>
+      <c r="L62">
+        <v>3.638888888888889</v>
+      </c>
       <c r="M62">
         <v>0</v>
       </c>
@@ -4543,6 +4669,12 @@
       <c r="K64">
         <v>13</v>
       </c>
+      <c r="L64">
+        <v>3.638888888888889</v>
+      </c>
+      <c r="M64">
+        <v>0.5888888888888889</v>
+      </c>
       <c r="N64" t="s">
         <v>285</v>
       </c>
@@ -4587,6 +4719,9 @@
       <c r="K65">
         <v>3</v>
       </c>
+      <c r="L65">
+        <v>3.638888888888889</v>
+      </c>
       <c r="M65">
         <v>1</v>
       </c>
@@ -4634,6 +4769,9 @@
       <c r="K66">
         <v>14</v>
       </c>
+      <c r="L66">
+        <v>3.638888888888889</v>
+      </c>
       <c r="M66">
         <v>0</v>
       </c>
@@ -4681,6 +4819,9 @@
       <c r="K67">
         <v>14</v>
       </c>
+      <c r="L67">
+        <v>3.638888888888889</v>
+      </c>
       <c r="M67">
         <v>0</v>
       </c>
@@ -4728,6 +4869,9 @@
       <c r="K68">
         <v>8</v>
       </c>
+      <c r="L68">
+        <v>3.638888888888889</v>
+      </c>
       <c r="M68">
         <v>0</v>
       </c>
@@ -4775,6 +4919,9 @@
       <c r="K69">
         <v>9</v>
       </c>
+      <c r="L69">
+        <v>3.638888888888889</v>
+      </c>
       <c r="M69">
         <v>1</v>
       </c>
@@ -4822,6 +4969,9 @@
       <c r="K70">
         <v>16</v>
       </c>
+      <c r="L70">
+        <v>3.638888888888889</v>
+      </c>
       <c r="M70">
         <v>2</v>
       </c>
@@ -4869,6 +5019,9 @@
       <c r="K71">
         <v>10</v>
       </c>
+      <c r="L71">
+        <v>3.638888888888889</v>
+      </c>
       <c r="M71">
         <v>1</v>
       </c>
@@ -4963,6 +5116,12 @@
       <c r="K73">
         <v>9</v>
       </c>
+      <c r="L73">
+        <v>3.638888888888889</v>
+      </c>
+      <c r="M73">
+        <v>0.5888888888888889</v>
+      </c>
       <c r="N73" t="s">
         <v>297</v>
       </c>
@@ -5004,6 +5163,12 @@
       <c r="K74">
         <v>18</v>
       </c>
+      <c r="L74">
+        <v>3.638888888888889</v>
+      </c>
+      <c r="M74">
+        <v>0.5888888888888889</v>
+      </c>
       <c r="N74" t="s">
         <v>293</v>
       </c>
@@ -5045,6 +5210,9 @@
       <c r="K75">
         <v>64</v>
       </c>
+      <c r="L75">
+        <v>3.638888888888889</v>
+      </c>
       <c r="M75">
         <v>0</v>
       </c>
@@ -5092,6 +5260,9 @@
       <c r="K76">
         <v>64</v>
       </c>
+      <c r="L76">
+        <v>3.638888888888889</v>
+      </c>
       <c r="M76">
         <v>0</v>
       </c>
@@ -5139,6 +5310,9 @@
       <c r="K77">
         <v>7</v>
       </c>
+      <c r="L77">
+        <v>3.638888888888889</v>
+      </c>
       <c r="M77">
         <v>1</v>
       </c>
@@ -5186,6 +5360,12 @@
       <c r="K78">
         <v>9</v>
       </c>
+      <c r="L78">
+        <v>3.638888888888889</v>
+      </c>
+      <c r="M78">
+        <v>0.5888888888888889</v>
+      </c>
       <c r="N78" t="s">
         <v>286</v>
       </c>
@@ -5230,6 +5410,9 @@
       <c r="K79">
         <v>17</v>
       </c>
+      <c r="L79">
+        <v>3.638888888888889</v>
+      </c>
       <c r="M79">
         <v>0</v>
       </c>
@@ -5274,6 +5457,9 @@
       <c r="K80">
         <v>284</v>
       </c>
+      <c r="L80">
+        <v>3.638888888888889</v>
+      </c>
       <c r="M80">
         <v>0</v>
       </c>
@@ -5321,6 +5507,9 @@
       <c r="K81">
         <v>8</v>
       </c>
+      <c r="L81">
+        <v>3.638888888888889</v>
+      </c>
       <c r="M81">
         <v>0</v>
       </c>
@@ -5368,6 +5557,9 @@
       <c r="K82">
         <v>24</v>
       </c>
+      <c r="L82">
+        <v>3.638888888888889</v>
+      </c>
       <c r="M82">
         <v>1</v>
       </c>
@@ -5415,6 +5607,9 @@
       <c r="K83">
         <v>24</v>
       </c>
+      <c r="L83">
+        <v>3.638888888888889</v>
+      </c>
       <c r="M83">
         <v>1</v>
       </c>
@@ -5462,6 +5657,9 @@
       <c r="K84">
         <v>8</v>
       </c>
+      <c r="L84">
+        <v>3.638888888888889</v>
+      </c>
       <c r="M84">
         <v>0</v>
       </c>
@@ -5506,6 +5704,9 @@
       <c r="K85">
         <v>19</v>
       </c>
+      <c r="L85">
+        <v>3.638888888888889</v>
+      </c>
       <c r="M85">
         <v>2</v>
       </c>
@@ -5706,6 +5907,9 @@
       <c r="L89">
         <v>4</v>
       </c>
+      <c r="M89">
+        <v>0.5888888888888889</v>
+      </c>
       <c r="N89" t="s">
         <v>291</v>
       </c>
@@ -5891,6 +6095,9 @@
       <c r="K93">
         <v>8</v>
       </c>
+      <c r="L93">
+        <v>3.638888888888889</v>
+      </c>
       <c r="M93">
         <v>0</v>
       </c>
@@ -5935,6 +6142,9 @@
       <c r="K94">
         <v>10</v>
       </c>
+      <c r="L94">
+        <v>3.638888888888889</v>
+      </c>
       <c r="M94">
         <v>1</v>
       </c>
@@ -5982,6 +6192,9 @@
       <c r="K95">
         <v>22</v>
       </c>
+      <c r="L95">
+        <v>3.638888888888889</v>
+      </c>
       <c r="M95">
         <v>0</v>
       </c>
@@ -6029,6 +6242,9 @@
       <c r="K96">
         <v>13</v>
       </c>
+      <c r="L96">
+        <v>3.638888888888889</v>
+      </c>
       <c r="M96">
         <v>0</v>
       </c>
@@ -6076,6 +6292,9 @@
       <c r="K97">
         <v>7</v>
       </c>
+      <c r="L97">
+        <v>3.638888888888889</v>
+      </c>
       <c r="M97">
         <v>0</v>
       </c>
@@ -6123,6 +6342,9 @@
       <c r="K98">
         <v>0</v>
       </c>
+      <c r="L98">
+        <v>3.638888888888889</v>
+      </c>
       <c r="M98">
         <v>1</v>
       </c>
@@ -6170,6 +6392,9 @@
       <c r="K99">
         <v>2</v>
       </c>
+      <c r="L99">
+        <v>3.638888888888889</v>
+      </c>
       <c r="M99">
         <v>2</v>
       </c>
@@ -6267,6 +6492,9 @@
       <c r="K101">
         <v>11</v>
       </c>
+      <c r="L101">
+        <v>3.638888888888889</v>
+      </c>
       <c r="M101">
         <v>0</v>
       </c>
@@ -6314,6 +6542,12 @@
       <c r="K102">
         <v>8</v>
       </c>
+      <c r="L102">
+        <v>3.638888888888889</v>
+      </c>
+      <c r="M102">
+        <v>0.5888888888888889</v>
+      </c>
       <c r="N102" t="s">
         <v>286</v>
       </c>
@@ -6357,6 +6591,12 @@
       </c>
       <c r="K103">
         <v>21</v>
+      </c>
+      <c r="L103">
+        <v>3.638888888888889</v>
+      </c>
+      <c r="M103">
+        <v>0.5888888888888889</v>
       </c>
       <c r="N103" t="s">
         <v>300</v>

</xml_diff>

<commit_message>
Scaling bed time data to am/pm
</commit_message>
<xml_diff>
--- a/clean_data.xlsx
+++ b/clean_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1325" uniqueCount="380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1325" uniqueCount="376">
   <si>
     <t>Birth Country</t>
   </si>
@@ -910,25 +910,13 @@
     <t>01:00:00</t>
   </si>
   <si>
-    <t>22:00:00</t>
-  </si>
-  <si>
-    <t>23:30:00</t>
+    <t>11:30:00</t>
   </si>
   <si>
     <t>00:30:00</t>
   </si>
   <si>
-    <t>23:00:00</t>
-  </si>
-  <si>
-    <t>11:30:00</t>
-  </si>
-  <si>
     <t>01:10:00</t>
-  </si>
-  <si>
-    <t>21:00:00</t>
   </si>
   <si>
     <t>02:30:00</t>
@@ -1668,10 +1656,10 @@
         <v>279</v>
       </c>
       <c r="O3" t="s">
-        <v>290</v>
+        <v>296</v>
       </c>
       <c r="P3" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -1721,7 +1709,7 @@
         <v>296</v>
       </c>
       <c r="P4" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -1771,7 +1759,7 @@
         <v>297</v>
       </c>
       <c r="P5" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -1865,7 +1853,7 @@
         <v>296</v>
       </c>
       <c r="P7" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -1912,10 +1900,10 @@
         <v>279</v>
       </c>
       <c r="O8" t="s">
-        <v>298</v>
+        <v>278</v>
       </c>
       <c r="P8" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -1962,10 +1950,10 @@
         <v>280</v>
       </c>
       <c r="O9" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="P9" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -2012,10 +2000,10 @@
         <v>280</v>
       </c>
       <c r="O10" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="P10" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
     </row>
     <row r="11" spans="1:16">
@@ -2065,7 +2053,7 @@
         <v>296</v>
       </c>
       <c r="P11" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
     </row>
     <row r="12" spans="1:16">
@@ -2112,7 +2100,7 @@
         <v>279</v>
       </c>
       <c r="O12" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
     </row>
     <row r="13" spans="1:16">
@@ -2162,7 +2150,7 @@
         <v>297</v>
       </c>
       <c r="P13" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
     </row>
     <row r="14" spans="1:16">
@@ -2212,7 +2200,7 @@
         <v>296</v>
       </c>
       <c r="P14" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
     </row>
     <row r="15" spans="1:16">
@@ -2262,7 +2250,7 @@
         <v>297</v>
       </c>
       <c r="P15" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
     </row>
     <row r="16" spans="1:16">
@@ -2309,10 +2297,10 @@
         <v>283</v>
       </c>
       <c r="O16" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="P16" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
     </row>
     <row r="17" spans="1:16">
@@ -2362,7 +2350,7 @@
         <v>297</v>
       </c>
       <c r="P17" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
     </row>
     <row r="18" spans="1:16">
@@ -2456,7 +2444,7 @@
         <v>297</v>
       </c>
       <c r="P19" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
     </row>
     <row r="20" spans="1:16">
@@ -2506,7 +2494,7 @@
         <v>297</v>
       </c>
       <c r="P20" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
     </row>
     <row r="21" spans="1:16">
@@ -2553,10 +2541,10 @@
         <v>285</v>
       </c>
       <c r="O21" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="P21" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
     </row>
     <row r="22" spans="1:16">
@@ -2603,7 +2591,7 @@
         <v>297</v>
       </c>
       <c r="P22" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
     </row>
     <row r="23" spans="1:16">
@@ -2647,7 +2635,7 @@
         <v>280</v>
       </c>
       <c r="O23" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="24" spans="1:16">
@@ -2691,7 +2679,7 @@
         <v>280</v>
       </c>
       <c r="O24" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="25" spans="1:16">
@@ -2738,10 +2726,10 @@
         <v>286</v>
       </c>
       <c r="O25" t="s">
-        <v>304</v>
+        <v>280</v>
       </c>
       <c r="P25" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
     </row>
     <row r="26" spans="1:16">
@@ -2788,10 +2776,10 @@
         <v>287</v>
       </c>
       <c r="O26" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="P26" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
     </row>
     <row r="27" spans="1:16">
@@ -2838,10 +2826,10 @@
         <v>288</v>
       </c>
       <c r="O27" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="P27" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
     </row>
     <row r="28" spans="1:16">
@@ -2888,7 +2876,7 @@
         <v>278</v>
       </c>
       <c r="O28" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
     </row>
     <row r="29" spans="1:16">
@@ -2935,10 +2923,10 @@
         <v>280</v>
       </c>
       <c r="O29" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="P29" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
     </row>
     <row r="30" spans="1:16">
@@ -2985,10 +2973,10 @@
         <v>280</v>
       </c>
       <c r="O30" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="P30" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
     </row>
     <row r="31" spans="1:16">
@@ -3038,7 +3026,7 @@
         <v>297</v>
       </c>
       <c r="P31" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
     </row>
     <row r="32" spans="1:16">
@@ -3085,10 +3073,10 @@
         <v>278</v>
       </c>
       <c r="O32" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="P32" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
     </row>
     <row r="33" spans="1:16">
@@ -3135,10 +3123,10 @@
         <v>278</v>
       </c>
       <c r="O33" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="P33" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
     </row>
     <row r="34" spans="1:16">
@@ -3232,10 +3220,10 @@
         <v>280</v>
       </c>
       <c r="O35" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="P35" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
     </row>
     <row r="36" spans="1:16">
@@ -3285,7 +3273,7 @@
         <v>297</v>
       </c>
       <c r="P36" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
     </row>
     <row r="37" spans="1:16">
@@ -3335,7 +3323,7 @@
         <v>297</v>
       </c>
       <c r="P37" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
     </row>
     <row r="38" spans="1:16">
@@ -3382,10 +3370,10 @@
         <v>289</v>
       </c>
       <c r="O38" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="P38" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="39" spans="1:16">
@@ -3476,10 +3464,10 @@
         <v>279</v>
       </c>
       <c r="O40" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="P40" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
     </row>
     <row r="41" spans="1:16">
@@ -3526,10 +3514,10 @@
         <v>279</v>
       </c>
       <c r="O41" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="P41" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
     </row>
     <row r="42" spans="1:16">
@@ -3579,7 +3567,7 @@
         <v>296</v>
       </c>
       <c r="P42" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
     </row>
     <row r="43" spans="1:16">
@@ -3626,7 +3614,7 @@
         <v>296</v>
       </c>
       <c r="P43" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
     </row>
     <row r="44" spans="1:16">
@@ -3676,7 +3664,7 @@
         <v>296</v>
       </c>
       <c r="P44" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
     </row>
     <row r="45" spans="1:16">
@@ -3726,7 +3714,7 @@
         <v>296</v>
       </c>
       <c r="P45" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
     </row>
     <row r="46" spans="1:16">
@@ -3776,7 +3764,7 @@
         <v>297</v>
       </c>
       <c r="P46" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
     </row>
     <row r="47" spans="1:16">
@@ -3826,7 +3814,7 @@
         <v>297</v>
       </c>
       <c r="P47" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
     </row>
     <row r="48" spans="1:16">
@@ -3873,10 +3861,10 @@
         <v>280</v>
       </c>
       <c r="O48" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="P48" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
     </row>
     <row r="49" spans="1:16">
@@ -3926,7 +3914,7 @@
         <v>297</v>
       </c>
       <c r="P49" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
     </row>
     <row r="50" spans="1:16">
@@ -3973,7 +3961,7 @@
         <v>296</v>
       </c>
       <c r="P50" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
     </row>
     <row r="51" spans="1:16">
@@ -4023,7 +4011,7 @@
         <v>296</v>
       </c>
       <c r="P51" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
     </row>
     <row r="52" spans="1:16">
@@ -4073,7 +4061,7 @@
         <v>297</v>
       </c>
       <c r="P52" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
     </row>
     <row r="53" spans="1:16">
@@ -4120,7 +4108,7 @@
         <v>297</v>
       </c>
       <c r="P53" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
     </row>
     <row r="54" spans="1:16">
@@ -4170,7 +4158,7 @@
         <v>296</v>
       </c>
       <c r="P54" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
     </row>
     <row r="55" spans="1:16">
@@ -4217,10 +4205,10 @@
         <v>288</v>
       </c>
       <c r="O55" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="P55" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
     </row>
     <row r="56" spans="1:16">
@@ -4267,10 +4255,10 @@
         <v>288</v>
       </c>
       <c r="O56" t="s">
-        <v>290</v>
+        <v>296</v>
       </c>
       <c r="P56" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
     </row>
     <row r="57" spans="1:16">
@@ -4320,7 +4308,7 @@
         <v>293</v>
       </c>
       <c r="P57" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
     </row>
     <row r="58" spans="1:16">
@@ -4367,10 +4355,10 @@
         <v>291</v>
       </c>
       <c r="O58" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="P58" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
     </row>
     <row r="59" spans="1:16">
@@ -4417,7 +4405,7 @@
         <v>278</v>
       </c>
       <c r="O59" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
     </row>
     <row r="60" spans="1:16">
@@ -4464,10 +4452,10 @@
         <v>279</v>
       </c>
       <c r="O60" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="P60" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
     </row>
     <row r="61" spans="1:16">
@@ -4514,7 +4502,7 @@
         <v>296</v>
       </c>
       <c r="P61" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
     </row>
     <row r="62" spans="1:16">
@@ -4608,10 +4596,10 @@
         <v>286</v>
       </c>
       <c r="O63" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="P63" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
     </row>
     <row r="64" spans="1:16">
@@ -4658,10 +4646,10 @@
         <v>278</v>
       </c>
       <c r="O64" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="P64" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
     </row>
     <row r="65" spans="1:16">
@@ -4711,7 +4699,7 @@
         <v>297</v>
       </c>
       <c r="P65" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
     </row>
     <row r="66" spans="1:16">
@@ -4758,10 +4746,10 @@
         <v>288</v>
       </c>
       <c r="O66" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="P66" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
     </row>
     <row r="67" spans="1:16">
@@ -4808,10 +4796,10 @@
         <v>288</v>
       </c>
       <c r="O67" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="P67" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
     </row>
     <row r="68" spans="1:16">
@@ -4861,7 +4849,7 @@
         <v>297</v>
       </c>
       <c r="P68" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
     </row>
     <row r="69" spans="1:16">
@@ -4908,10 +4896,10 @@
         <v>278</v>
       </c>
       <c r="O69" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="P69" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
     </row>
     <row r="70" spans="1:16">
@@ -4958,10 +4946,10 @@
         <v>286</v>
       </c>
       <c r="O70" t="s">
-        <v>290</v>
+        <v>296</v>
       </c>
       <c r="P70" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
     </row>
     <row r="71" spans="1:16">
@@ -5011,7 +4999,7 @@
         <v>296</v>
       </c>
       <c r="P71" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
     </row>
     <row r="72" spans="1:16">
@@ -5061,7 +5049,7 @@
         <v>297</v>
       </c>
       <c r="P72" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="73" spans="1:16">
@@ -5202,7 +5190,7 @@
         <v>297</v>
       </c>
       <c r="P75" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
     </row>
     <row r="76" spans="1:16">
@@ -5252,7 +5240,7 @@
         <v>297</v>
       </c>
       <c r="P76" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
     </row>
     <row r="77" spans="1:16">
@@ -5302,7 +5290,7 @@
         <v>296</v>
       </c>
       <c r="P77" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
     </row>
     <row r="78" spans="1:16">
@@ -5352,7 +5340,7 @@
         <v>296</v>
       </c>
       <c r="P78" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
     </row>
     <row r="79" spans="1:16">
@@ -5399,10 +5387,10 @@
         <v>287</v>
       </c>
       <c r="O79" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="P79" s="2" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
     </row>
     <row r="80" spans="1:16">
@@ -5449,7 +5437,7 @@
         <v>297</v>
       </c>
       <c r="P80" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
     </row>
     <row r="81" spans="1:16">
@@ -5496,10 +5484,10 @@
         <v>279</v>
       </c>
       <c r="O81" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="P81" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
     </row>
     <row r="82" spans="1:16">
@@ -5546,10 +5534,10 @@
         <v>278</v>
       </c>
       <c r="O82" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="P82" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
     </row>
     <row r="83" spans="1:16">
@@ -5596,10 +5584,10 @@
         <v>278</v>
       </c>
       <c r="O83" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="P83" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
     </row>
     <row r="84" spans="1:16">
@@ -5693,10 +5681,10 @@
         <v>287</v>
       </c>
       <c r="O85" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="P85" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
     </row>
     <row r="86" spans="1:16">
@@ -5746,7 +5734,7 @@
         <v>296</v>
       </c>
       <c r="P86" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
     </row>
     <row r="87" spans="1:16">
@@ -5796,7 +5784,7 @@
         <v>297</v>
       </c>
       <c r="P87" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
     </row>
     <row r="88" spans="1:16">
@@ -5846,7 +5834,7 @@
         <v>297</v>
       </c>
       <c r="P88" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
     </row>
     <row r="89" spans="1:16">
@@ -5896,7 +5884,7 @@
         <v>296</v>
       </c>
       <c r="P89" s="2" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
     </row>
     <row r="90" spans="1:16">
@@ -5940,7 +5928,7 @@
         <v>293</v>
       </c>
       <c r="O90" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
     </row>
     <row r="91" spans="1:16">
@@ -5990,7 +5978,7 @@
         <v>296</v>
       </c>
       <c r="P91" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
     </row>
     <row r="92" spans="1:16">
@@ -6037,10 +6025,10 @@
         <v>280</v>
       </c>
       <c r="O92" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="P92" s="2" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
     </row>
     <row r="93" spans="1:16">
@@ -6131,10 +6119,10 @@
         <v>284</v>
       </c>
       <c r="O94" t="s">
-        <v>298</v>
+        <v>278</v>
       </c>
       <c r="P94" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
     </row>
     <row r="95" spans="1:16">
@@ -6181,10 +6169,10 @@
         <v>283</v>
       </c>
       <c r="O95" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="P95" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
     </row>
     <row r="96" spans="1:16">
@@ -6231,10 +6219,10 @@
         <v>278</v>
       </c>
       <c r="O96" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="P96" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
     </row>
     <row r="97" spans="1:16">
@@ -6281,10 +6269,10 @@
         <v>294</v>
       </c>
       <c r="O97" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="P97" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
     </row>
     <row r="98" spans="1:16">
@@ -6334,7 +6322,7 @@
         <v>297</v>
       </c>
       <c r="P98" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
     </row>
     <row r="99" spans="1:16">
@@ -6384,7 +6372,7 @@
         <v>297</v>
       </c>
       <c r="P99" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
     </row>
     <row r="100" spans="1:16">
@@ -6434,7 +6422,7 @@
         <v>296</v>
       </c>
       <c r="P100" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
     </row>
     <row r="101" spans="1:16">
@@ -6481,10 +6469,10 @@
         <v>278</v>
       </c>
       <c r="O101" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="P101" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
     </row>
     <row r="102" spans="1:16">
@@ -6534,7 +6522,7 @@
         <v>297</v>
       </c>
       <c r="P102" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
     </row>
     <row r="103" spans="1:16">
@@ -6581,10 +6569,10 @@
         <v>293</v>
       </c>
       <c r="O103" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="P103" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
     </row>
     <row r="104" spans="1:16">
@@ -6631,10 +6619,10 @@
         <v>295</v>
       </c>
       <c r="O104" t="s">
-        <v>304</v>
+        <v>280</v>
       </c>
       <c r="P104" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
     </row>
   </sheetData>

</xml_diff>